<commit_message>
bug list and license service ref removal
</commit_message>
<xml_diff>
--- a/release-notes/11-2022/closed-bugs-sle-11-2022.xlsx
+++ b/release-notes/11-2022/closed-bugs-sle-11-2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markblack/repos/github/install-systemlink-enterprise/release-notes/11-2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC080C4-B233-9B49-8158-38AC91F7DBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDEDFC6-2201-A245-BB37-FDB6E3798424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -34,9 +34,6 @@
     <t>State</t>
   </si>
   <si>
-    <t>Tags</t>
-  </si>
-  <si>
     <t>Bug</t>
   </si>
   <si>
@@ -46,33 +43,18 @@
     <t>[XRAY] Update bitnami/rabbitmq:3.10.7-debian-11-r11 to r17</t>
   </si>
   <si>
-    <t>CustomerFacing</t>
-  </si>
-  <si>
     <t>[XRAY] Update bitnami/redis-cluster:7.0.4-debian-11-r14 to r17</t>
   </si>
   <si>
     <t>[XRAY] Update kiwigrid/k8s-sidecar:1.19.2 to 1.19.5</t>
   </si>
   <si>
-    <t>C3-09; CustomerFacing</t>
-  </si>
-  <si>
-    <t>Apparent data integrity issue with DFS</t>
-  </si>
-  <si>
-    <t>C4-10</t>
-  </si>
-  <si>
     <t>Breadcrumb behavior | The breadcrumb is not updating properly if the url contains query parameters</t>
   </si>
   <si>
     <t xml:space="preserve">Create / Product requires 'Name' field, should not be required. </t>
   </si>
   <si>
-    <t>NotCustomerFacing; Reviewed</t>
-  </si>
-  <si>
     <t>Create Steps | Fails when input/output field values are null</t>
   </si>
   <si>
@@ -82,24 +64,12 @@
     <t>Data tables Visualize link to Grafana Explore should open in a new browser tab</t>
   </si>
   <si>
-    <t>Reviewed</t>
-  </si>
-  <si>
     <t>Edit Product | Sporadic - Editing a valid product throws error</t>
   </si>
   <si>
-    <t>Edit Product from UI | Minor lag is updating fields</t>
-  </si>
-  <si>
-    <t>Edited file name does not get reflected in the grid</t>
-  </si>
-  <si>
     <t>Expanded view controls are not scrollable when longer than page height</t>
   </si>
   <si>
-    <t>Group Hidden Columns</t>
-  </si>
-  <si>
     <t>KafkaRowDataWriter transactional IDs may not be unique across pods</t>
   </si>
   <si>
@@ -125,6 +95,33 @@
   </si>
   <si>
     <t>Update RabbitMQ Helm Chart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[XRAY - nbparsingservice, nbexecworker, jupyter-notebook-userpod] Make base image tag more specific </t>
+  </si>
+  <si>
+    <t>All SLE users can see policies IDs and entitlements for all other users in the same org</t>
+  </si>
+  <si>
+    <t>[XRAY - GM reported] zookeeper:3.8.0</t>
+  </si>
+  <si>
+    <t>[XRAY - GM reported] kiwigrid/k8s-sidecar:1.19.5</t>
+  </si>
+  <si>
+    <t>[XRAY - GM reported] ni/systemlink/dataframeservice-kafka-connect:20221020.2</t>
+  </si>
+  <si>
+    <t>[XRAY - GM reported] bitnami/schema-registry</t>
+  </si>
+  <si>
+    <t>Concurrent writes to single data table can lead to dropped rows</t>
+  </si>
+  <si>
+    <t>Product Details | Edited file name does not get reflected in the grid</t>
+  </si>
+  <si>
+    <t>Need to support Group by Hidden Columns</t>
   </si>
 </sst>
 </file>
@@ -965,19 +962,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="122.33203125" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" customWidth="1"/>
+    <col min="4" max="4" width="60.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -990,357 +987,425 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2159209</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2159211</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2159247</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2194467</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2177045</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2150495</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2171177</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2195427</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2162736</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2195438</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2176471</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2116831</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2180695</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2192043</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2176468</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2167479</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2119196</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2145644</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2192619</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
         <v>21</v>
       </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>2195515</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2181700</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
         <v>22</v>
       </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>2176471</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2047675</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>2116831</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2159327</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
         <v>24</v>
       </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>2180695</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2156702</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
         <v>25</v>
       </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>2192043</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2171852</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
         <v>26</v>
       </c>
-      <c r="D16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>2176468</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2193592</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
         <v>27</v>
       </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>2167479</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2193582</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
         <v>28</v>
       </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>2119196</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2193574</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
         <v>29</v>
       </c>
-      <c r="D19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>2145644</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2193554</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
         <v>30</v>
       </c>
-      <c r="D20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>2192619</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
         <v>2181700</v>
       </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>2047675</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>2159327</v>
-      </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" t="s">
-        <v>6</v>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2171177</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>